<commit_message>
new file:   ctcc/main.cpp new file:   ctcc/tokeniser.h
</commit_message>
<xml_diff>
--- a/ce-cbc-spec.xlsx
+++ b/ce-cbc-spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/Documents/ctc-lang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72EBFB4E-627A-FA46-AE40-8AE7FDDDA35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B8B3FF-C8B3-E74D-89BE-99411B19EEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25720" yWindow="480" windowWidth="25480" windowHeight="28320" xr2:uid="{E91755C5-3C5B-2246-954C-C569B4044A2E}"/>
+    <workbookView minimized="1" xWindow="11880" yWindow="5860" windowWidth="28040" windowHeight="17440" xr2:uid="{E91755C5-3C5B-2246-954C-C569B4044A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="96">
   <si>
     <t>Text</t>
   </si>
@@ -168,6 +168,162 @@
   </si>
   <si>
     <t>CODE</t>
+  </si>
+  <si>
+    <t>SI32</t>
+  </si>
+  <si>
+    <t>SI64</t>
+  </si>
+  <si>
+    <t>SU32</t>
+  </si>
+  <si>
+    <t>SU64</t>
+  </si>
+  <si>
+    <t>SF32</t>
+  </si>
+  <si>
+    <t>SF64</t>
+  </si>
+  <si>
+    <t>AI32</t>
+  </si>
+  <si>
+    <t>AI64</t>
+  </si>
+  <si>
+    <t>AU32</t>
+  </si>
+  <si>
+    <t>AU64</t>
+  </si>
+  <si>
+    <t>AF32</t>
+  </si>
+  <si>
+    <t>AF64</t>
+  </si>
+  <si>
+    <t>MI32</t>
+  </si>
+  <si>
+    <t>MI64</t>
+  </si>
+  <si>
+    <t>MU32</t>
+  </si>
+  <si>
+    <t>MU64</t>
+  </si>
+  <si>
+    <t>MF32</t>
+  </si>
+  <si>
+    <t>MF64</t>
+  </si>
+  <si>
+    <t>DI32</t>
+  </si>
+  <si>
+    <t>DI64</t>
+  </si>
+  <si>
+    <t>DU32</t>
+  </si>
+  <si>
+    <t>DU64</t>
+  </si>
+  <si>
+    <t>DF32</t>
+  </si>
+  <si>
+    <t>DF64</t>
+  </si>
+  <si>
+    <t>OI32</t>
+  </si>
+  <si>
+    <t>OI64</t>
+  </si>
+  <si>
+    <t>OU32</t>
+  </si>
+  <si>
+    <t>OU64</t>
+  </si>
+  <si>
+    <t>OF32</t>
+  </si>
+  <si>
+    <t>OF64</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>UI32</t>
+  </si>
+  <si>
+    <t>UI64</t>
+  </si>
+  <si>
+    <t>UU32</t>
+  </si>
+  <si>
+    <t>UU64</t>
+  </si>
+  <si>
+    <t>UF32</t>
+  </si>
+  <si>
+    <t>UF64</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>subtract</t>
+  </si>
+  <si>
+    <t>multiply</t>
+  </si>
+  <si>
+    <t>divide</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>JIFE</t>
+  </si>
+  <si>
+    <t>JIFN</t>
+  </si>
+  <si>
+    <t>jump by value</t>
+  </si>
+  <si>
+    <t>jump if current location is true</t>
+  </si>
+  <si>
+    <t>jump if current location == address</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>jump if current != address</t>
+  </si>
+  <si>
+    <t>move current to address</t>
+  </si>
+  <si>
+    <t>run function at address</t>
+  </si>
+  <si>
+    <t>run C function at address</t>
   </si>
 </sst>
 </file>
@@ -532,22 +688,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0EE3F5-3B8D-5640-B84B-48674F71BAF5}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -558,447 +714,992 @@
         <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61" s="1"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="1"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="1"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D86" s="1"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>